<commit_message>
stoch discounting to zero added
</commit_message>
<xml_diff>
--- a/Runfiles/RiskDriverSimulation/IRinput.xlsx
+++ b/Runfiles/RiskDriverSimulation/IRinput.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Risk Driver Simulation\Runfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Runfiles\RiskDriverSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB0A966-4F73-417C-891C-12DBC1ADF5F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6105535E-A763-4B23-96D5-379956EF59DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>foreign20</t>
+  </si>
+  <si>
+    <t>Discountcurve</t>
+  </si>
+  <si>
+    <t>USDOIS 31122019</t>
   </si>
 </sst>
 </file>
@@ -497,16 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,6 +626,14 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>